<commit_message>
Add new PCB version and update project files
Introduced Buck_Converter_PCB_9.PcbDoc and associated output files, updated Buck_Converter.PrjPcb to reference the new PCB, and modified schematic and PCB documents. Updated BOM and project output reports, and managed history files to reflect the new version.
</commit_message>
<xml_diff>
--- a/BOM list.xlsx
+++ b/BOM list.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81EF5241-407B-4F7A-B2DA-FF6352495073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_Designer_Project\Buck_Converter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D5401F-159B-425B-A060-CA85A8DF4A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{DBF4FEB7-C8F1-4AC9-92C9-0401681DC220}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DBF4FEB7-C8F1-4AC9-92C9-0401681DC220}"/>
   </bookViews>
   <sheets>
     <sheet name="Buck_Converter_PCB" sheetId="1" r:id="rId1"/>
@@ -132,127 +137,129 @@
     <t>PD1, PD2, PD3, PD4</t>
   </si>
   <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>2SCR552P</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>2SAR552P</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RESISTOR_SMD_0805</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>R2, R6, R12</t>
+  </si>
+  <si>
+    <t>3K</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>R4, R8, R18</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>24K</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>22R</t>
+  </si>
+  <si>
+    <t>R9, R10</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>0R01</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>RESISTOR_SMD_2512</t>
+  </si>
+  <si>
+    <t>15K</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>1K5</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>4R7</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>RESISTOR_SMD_1206</t>
+  </si>
+  <si>
+    <t>TL494CDR</t>
+  </si>
+  <si>
+    <t>B78307A2276A003</t>
+  </si>
+  <si>
+    <t>TR1</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>VR1, VR2</t>
+  </si>
+  <si>
+    <t>Baoter_3296</t>
+  </si>
+  <si>
+    <t>TO-220N-MOSFET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>N-MOSFET</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>TO-220)N-MOSFET</t>
-  </si>
-  <si>
-    <t>2SCR552P</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>2SAR552P</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>RESISTOR_SMD_0805</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>R2, R6, R12</t>
-  </si>
-  <si>
-    <t>3K</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>R4, R8, R18</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>24K</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>22R</t>
-  </si>
-  <si>
-    <t>R9, R10</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>0R01</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>RESISTOR_SMD_2512</t>
-  </si>
-  <si>
-    <t>15K</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>1K5</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>4R7</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>RESISTOR_SMD_1206</t>
-  </si>
-  <si>
-    <t>TL494CDR</t>
-  </si>
-  <si>
-    <t>B78307A2276A003</t>
-  </si>
-  <si>
-    <t>TR1</t>
-  </si>
-  <si>
-    <t>5K</t>
-  </si>
-  <si>
-    <t>VR1, VR2</t>
-  </si>
-  <si>
-    <t>Baoter_3296</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -674,11 +681,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9517768C-E708-44AA-ACC9-6E9FCDAE713A}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -865,13 +877,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
@@ -879,13 +891,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -893,13 +905,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -907,13 +919,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
@@ -921,13 +933,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="3">
         <v>3</v>
@@ -935,13 +947,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -949,13 +961,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20" s="3">
         <v>3</v>
@@ -963,13 +975,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -977,13 +989,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -991,13 +1003,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" s="3">
         <v>2</v>
@@ -1005,13 +1017,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -1019,13 +1031,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -1033,13 +1045,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -1047,13 +1059,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -1061,13 +1073,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -1075,13 +1087,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -1089,13 +1101,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -1103,13 +1115,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -1117,13 +1129,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D32" s="3">
         <v>2</v>

</xml_diff>